<commit_message>
JS basics and exercises
</commit_message>
<xml_diff>
--- a/Programming Basics-C#/ProgrammingNotes.xlsx
+++ b/Programming Basics-C#/ProgrammingNotes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SoftUniQA-Courses\Programming Basics-C#\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED28B428-ABD4-40C8-BC0D-8AFC36FDB28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAF5974-E45D-4F09-8BB3-CA0913A6B33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="394">
   <si>
     <t>SELECT</t>
   </si>
@@ -1887,6 +1887,117 @@
   </si>
   <si>
     <t>converts string to the given type</t>
+  </si>
+  <si>
+    <t>STRING specifics</t>
+  </si>
+  <si>
+    <t>char[] charArray = var.ToCharArray()</t>
+  </si>
+  <si>
+    <t>converting string into char array</t>
+  </si>
+  <si>
+    <t>string text = "text"</t>
+  </si>
+  <si>
+    <t>char[] charArray = text.ToCharArray() // ['t', 'e', 'x', 't']</t>
+  </si>
+  <si>
+    <t>concatenates strings method</t>
+  </si>
+  <si>
+    <t>string greet = "hello, "    string name = "George"</t>
+  </si>
+  <si>
+    <t>string result = string.Contact( greet, name)  // Hello, George</t>
+  </si>
+  <si>
+    <t>string.Contact()</t>
+  </si>
+  <si>
+    <t>IndexOf()</t>
+  </si>
+  <si>
+    <t>returns the first match index or -1</t>
+  </si>
+  <si>
+    <t>string fruits = "banana, apple, kiwi"</t>
+  </si>
+  <si>
+    <t>(fruits.IndexOf("banana")) // 0    first letter b is on index# 0</t>
+  </si>
+  <si>
+    <t>LastIndexOf()</t>
+  </si>
+  <si>
+    <t>returns last match index occurance</t>
+  </si>
+  <si>
+    <t>string fruits = "banana, apple, kiwi, banana, apple"</t>
+  </si>
+  <si>
+    <t>(fruits.IndexOf("banana")) //21    first letter b is on index# 0 from back to forward</t>
+  </si>
+  <si>
+    <t>Contains()</t>
+  </si>
+  <si>
+    <t>bool. Finds a string if is contained in a string var</t>
+  </si>
+  <si>
+    <t>string text = "I love fruits"</t>
+  </si>
+  <si>
+    <t>(text.Contains("fruits"))  - will return True as the string contains the word</t>
+  </si>
+  <si>
+    <t>Substring(int startIndex, int length)</t>
+  </si>
+  <si>
+    <t>string card = "10C"</t>
+  </si>
+  <si>
+    <t>string power = card.Substring(0, 2)  // 10</t>
+  </si>
+  <si>
+    <t>Substring(int startIndex)</t>
+  </si>
+  <si>
+    <t>string name = "My name is John"   (name starts at the 11th index)</t>
+  </si>
+  <si>
+    <t>string exactName = string.Substring(11)  // returns John</t>
+  </si>
+  <si>
+    <t>Replace(match, replacement)</t>
+  </si>
+  <si>
+    <t>replaces a matched string with a new one</t>
+  </si>
+  <si>
+    <t>.Replace(ggajev1@abv.bg, gadzhev@abv.bg) // new string will be gadzhev@abv.bg</t>
+  </si>
+  <si>
+    <t>replacement text should be same string length</t>
+  </si>
+  <si>
+    <t>StringBuilder sb = new StringBuilder()</t>
+  </si>
+  <si>
+    <t>build/modify strings class</t>
+  </si>
+  <si>
+    <t>sb.Append</t>
+  </si>
+  <si>
+    <t>Stopwatch sw = new Stopwatch()</t>
+  </si>
+  <si>
+    <t>sw.Start()</t>
+  </si>
+  <si>
+    <t>(sw.ElapsedMilliSeconds)</t>
   </si>
 </sst>
 </file>
@@ -2286,7 +2397,7 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -3723,17 +3834,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E2E049-E1BB-4C51-B7AA-1C5399BF770F}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.28515625" customWidth="1"/>
     <col min="2" max="2" width="51.42578125" customWidth="1"/>
-    <col min="3" max="3" width="65" customWidth="1"/>
+    <col min="3" max="3" width="77.5703125" customWidth="1"/>
     <col min="4" max="4" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4444,6 +4555,161 @@
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
         <v>355</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>358</v>
+      </c>
+      <c r="B95" t="s">
+        <v>359</v>
+      </c>
+      <c r="C95" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>365</v>
+      </c>
+      <c r="B98" t="s">
+        <v>362</v>
+      </c>
+      <c r="C98" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>366</v>
+      </c>
+      <c r="B101" t="s">
+        <v>367</v>
+      </c>
+      <c r="C101" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>370</v>
+      </c>
+      <c r="B104" t="s">
+        <v>371</v>
+      </c>
+      <c r="C104" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>374</v>
+      </c>
+      <c r="B107" t="s">
+        <v>375</v>
+      </c>
+      <c r="C107" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>378</v>
+      </c>
+      <c r="C110" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>381</v>
+      </c>
+      <c r="C113" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>384</v>
+      </c>
+      <c r="B116" t="s">
+        <v>385</v>
+      </c>
+      <c r="C116" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>388</v>
+      </c>
+      <c r="B120" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>